<commit_message>
- Actually fix xlsx support - Add collated output for summary table and CNV calls
</commit_message>
<xml_diff>
--- a/tests/data/sample_table.xlsx
+++ b/tests/data/sample_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t xml:space="preserve">Array_Name</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cellline-A MasterBank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cellline-A-WB,Cellline-B-MB</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -121,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,8 +184,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,183 +213,183 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>123456789000</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="H3" s="1" t="n">
+        <v>123456789001</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>123456789000</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>123456789000</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>123456789001</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>123456789000</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>123456789000</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>123456789001</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>28</v>
+      <c r="J6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>